<commit_message>
popravljen opis primerov uporabe
</commit_message>
<xml_diff>
--- a/frontend/opisPrimerovUporabe.xlsx
+++ b/frontend/opisPrimerovUporabe.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kitak\OneDrive\Desktop\RIS\frontend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\RIS\frontend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B458E6-B892-4456-9198-9833319CED8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F340650-DD96-4555-9373-9518EAB486A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="83">
   <si>
     <t>Atribut</t>
   </si>
@@ -61,9 +61,6 @@
     <t>PU4</t>
   </si>
   <si>
-    <t>PU4a</t>
-  </si>
-  <si>
     <t>PU5</t>
   </si>
   <si>
@@ -88,9 +85,6 @@
     <t>Prikazati seznam vseh receptov in omogočiti vpogled v njihove podrobnosti.</t>
   </si>
   <si>
-    <t>Dovoliti Uporabniku, da svojemu receptu pripiše oceno za osebno evidenco.</t>
-  </si>
-  <si>
     <t>Posodabljanje vseh uporabniških računov, vključno z vlogami in statusi.</t>
   </si>
   <si>
@@ -124,9 +118,6 @@
     <t>Uporabnik je prijavljen ali neprijavljen (javni dostop).</t>
   </si>
   <si>
-    <t>Pregledani recept mora biti v lasti Uporabnika, ki ga pregleduje.</t>
-  </si>
-  <si>
     <t>Administrator je prijavljen.</t>
   </si>
   <si>
@@ -145,9 +136,6 @@
     <t>Stanje ostaja enako (le branje podatkov).</t>
   </si>
   <si>
-    <t>Shranjena je nova ocena za recept.</t>
-  </si>
-  <si>
     <t>Podatki o uporabniških računov so posodobljeni.</t>
   </si>
   <si>
@@ -166,9 +154,6 @@
     <t>1. Uporabnik izbere 'Pregled receptov'. 2. Sistem prikaže seznam. 3. Uporabnik klikne na recept za podrobnosti. 4. Če je Uporabnik lastnik, Sistem omogoči izvedbo PU4a.</t>
   </si>
   <si>
-    <t>1. Uporabnik vidi možnost ocenjevanja in vnese oceno (1-5). 2. Uporabnik klikne "Potrdi oceno". 3. Sistem shrani novo oceno.</t>
-  </si>
-  <si>
     <t>1. Administrator izbere "Upravljanje uporabnikov". 2. Administrator izbere uporabnika na seznamu. 3. Administrator spremeni vlogo/status/geslo. 4. Administrator shrani spremembe.</t>
   </si>
   <si>
@@ -190,9 +175,6 @@
     <t>2a. Uporabnik uporabi filtriranje po žanru.</t>
   </si>
   <si>
-    <t>PU4a ni poklican (Če recept ni Uporabnikov, se možnost ocenjevanja ne prikaže).</t>
-  </si>
-  <si>
     <t>3a. Administrator ustvari novega uporabnika z vlogo 'Moderator'.</t>
   </si>
   <si>
@@ -208,9 +190,6 @@
     <t>Izjema 1: Recept je označen kot zaščiten. Sistem prepreči brisanje z opozorilom.</t>
   </si>
   <si>
-    <t>Izjema 1: Uporabnik po pomoti poskuša oceniti dvakrat. Sistem javi: "Recept je že ocenjen s strani lastnika."</t>
-  </si>
-  <si>
     <t>Izjema 1: Administrator poskuša brisati lastni Administratorski račun. Sistem prepreči brisanje.</t>
   </si>
   <si>
@@ -236,9 +215,6 @@
   </si>
   <si>
     <t>Izjema 1: Povezava s PB je prekinjena. Sistem prikaže napako.</t>
-  </si>
-  <si>
-    <t>Uporabnik: OCENJEVANJE LASTNEGA RECEPTA (extend PU4)</t>
   </si>
   <si>
     <t>Uporabnik: IZBIRA KATEGORIJE (include v PU1)</t>
@@ -573,10 +549,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -587,14 +563,13 @@
     <col min="4" max="4" width="107.44140625" customWidth="1"/>
     <col min="5" max="5" width="104.44140625" customWidth="1"/>
     <col min="6" max="6" width="138.88671875" customWidth="1"/>
-    <col min="7" max="7" width="103.109375" customWidth="1"/>
-    <col min="8" max="8" width="146.77734375" customWidth="1"/>
-    <col min="9" max="9" width="127.88671875" customWidth="1"/>
-    <col min="10" max="10" width="142.77734375" customWidth="1"/>
-    <col min="11" max="11" width="38.88671875" customWidth="1"/>
+    <col min="7" max="7" width="146.77734375" customWidth="1"/>
+    <col min="8" max="8" width="127.88671875" customWidth="1"/>
+    <col min="9" max="9" width="142.77734375" customWidth="1"/>
+    <col min="10" max="10" width="38.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -602,7 +577,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -614,22 +589,19 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>72</v>
+        <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="I1" t="s">
+        <v>67</v>
+      </c>
       <c r="J1" t="s">
-        <v>75</v>
-      </c>
-      <c r="K1" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -654,259 +626,235 @@
       <c r="H2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J2" t="s">
-        <v>77</v>
-      </c>
-      <c r="K2" t="s">
-        <v>78</v>
+      <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>71</v>
+      </c>
+      <c r="J3" t="s">
+        <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="1" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J3" t="s">
-        <v>79</v>
-      </c>
-      <c r="K3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="C4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>26</v>
       </c>
       <c r="H4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K4" t="s">
-        <v>26</v>
+      <c r="D5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" t="s">
+        <v>73</v>
+      </c>
+      <c r="J5" t="s">
+        <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="1" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="J5" t="s">
+      <c r="I6" t="s">
+        <v>75</v>
+      </c>
+      <c r="J6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7" t="s">
+        <v>77</v>
+      </c>
+      <c r="J7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I8" t="s">
+        <v>79</v>
+      </c>
+      <c r="J8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I9" t="s">
         <v>81</v>
       </c>
-      <c r="K5" t="s">
+      <c r="J9" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="J6" t="s">
-        <v>83</v>
-      </c>
-      <c r="K6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J7" t="s">
-        <v>85</v>
-      </c>
-      <c r="K7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="J8" t="s">
-        <v>87</v>
-      </c>
-      <c r="K8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J9" t="s">
-        <v>89</v>
-      </c>
-      <c r="K9" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>